<commit_message>
changed the university name from german to english
</commit_message>
<xml_diff>
--- a/buehlot/metadata.xlsx
+++ b/buehlot/metadata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\flori\Documents\GitHub\scripts\buehlot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C15BD8F-A6AD-456F-99E1-85B7491DAE06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3995A3C-C8F8-4DF1-A2EB-BA273F941D1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{682A4A4C-CED8-4332-820B-8D70A758E6DF}"/>
   </bookViews>
@@ -219,10 +219,6 @@
     <t>OTT CTD</t>
   </si>
   <si>
-    <t>Karlsruher Institut für Technologie 
-(KIT)</t>
-  </si>
-  <si>
     <t>A precipitation gauge has sensors for two variables, one for the precipitation and one for the air temperature. The gauges are located in different areas to collect the data.</t>
   </si>
   <si>
@@ -458,6 +454,10 @@
   <si>
     <t xml:space="preserve">5390987.467
 </t>
+  </si>
+  <si>
+    <t>Karlsruher Institut of Technology 
+(KIT)</t>
   </si>
 </sst>
 </file>
@@ -528,7 +528,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -537,12 +537,6 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -861,9 +855,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3BDE976-8A87-43CF-A983-F371A8BBADE6}">
   <dimension ref="A1:P75"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K58" sqref="K58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -889,7 +883,7 @@
         <v>8</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
@@ -898,25 +892,25 @@
         <v>1</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>80</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>81</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>3</v>
@@ -939,7 +933,7 @@
         <v>9</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>16</v>
@@ -948,32 +942,32 @@
         <v>17</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G2" s="2"/>
       <c r="H2" s="2" t="s">
         <v>41</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K2" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="L2" s="3" t="s">
         <v>45</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>46</v>
       </c>
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
       <c r="O2" s="2"/>
-      <c r="P2" s="4" t="s">
-        <v>84</v>
+      <c r="P2" s="2" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="3" spans="1:16" ht="43.5" x14ac:dyDescent="0.35">
@@ -981,7 +975,7 @@
         <v>9</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>18</v>
@@ -990,32 +984,32 @@
         <v>19</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G3" s="2"/>
       <c r="H3" s="2" t="s">
         <v>38</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K3" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="L3" s="3" t="s">
         <v>45</v>
-      </c>
-      <c r="L3" s="3" t="s">
-        <v>46</v>
       </c>
       <c r="M3" s="2"/>
       <c r="N3" s="2"/>
       <c r="O3" s="2"/>
-      <c r="P3" s="4" t="s">
-        <v>84</v>
+      <c r="P3" s="2" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="4" spans="1:16" ht="43.5" x14ac:dyDescent="0.35">
@@ -1023,7 +1017,7 @@
         <v>10</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>16</v>
@@ -1032,32 +1026,32 @@
         <v>17</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G4" s="2"/>
       <c r="H4" s="2" t="s">
         <v>41</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K4" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="L4" s="3" t="s">
         <v>45</v>
-      </c>
-      <c r="L4" s="3" t="s">
-        <v>46</v>
       </c>
       <c r="M4" s="2"/>
       <c r="N4" s="2"/>
       <c r="O4" s="2"/>
-      <c r="P4" s="4" t="s">
-        <v>84</v>
+      <c r="P4" s="2" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="5" spans="1:16" ht="43.5" x14ac:dyDescent="0.35">
@@ -1065,7 +1059,7 @@
         <v>10</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>18</v>
@@ -1074,32 +1068,32 @@
         <v>19</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G5" s="2"/>
       <c r="H5" s="2" t="s">
         <v>38</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K5" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="L5" s="3" t="s">
         <v>45</v>
-      </c>
-      <c r="L5" s="3" t="s">
-        <v>46</v>
       </c>
       <c r="M5" s="2"/>
       <c r="N5" s="2"/>
       <c r="O5" s="2"/>
-      <c r="P5" s="4" t="s">
-        <v>84</v>
+      <c r="P5" s="2" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="6" spans="1:16" ht="43.5" x14ac:dyDescent="0.35">
@@ -1107,7 +1101,7 @@
         <v>11</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>16</v>
@@ -1116,32 +1110,32 @@
         <v>17</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G6" s="2"/>
       <c r="H6" s="2" t="s">
         <v>41</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K6" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="L6" s="3" t="s">
         <v>45</v>
-      </c>
-      <c r="L6" s="3" t="s">
-        <v>46</v>
       </c>
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
       <c r="O6" s="2"/>
-      <c r="P6" s="4" t="s">
-        <v>84</v>
+      <c r="P6" s="2" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="7" spans="1:16" ht="43.5" x14ac:dyDescent="0.35">
@@ -1149,7 +1143,7 @@
         <v>11</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>18</v>
@@ -1158,32 +1152,32 @@
         <v>19</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G7" s="2"/>
       <c r="H7" s="2" t="s">
         <v>38</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K7" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="L7" s="3" t="s">
         <v>45</v>
-      </c>
-      <c r="L7" s="3" t="s">
-        <v>46</v>
       </c>
       <c r="M7" s="2"/>
       <c r="N7" s="2"/>
       <c r="O7" s="2"/>
-      <c r="P7" s="4" t="s">
-        <v>84</v>
+      <c r="P7" s="2" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="8" spans="1:16" ht="43.5" x14ac:dyDescent="0.35">
@@ -1191,7 +1185,7 @@
         <v>12</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>16</v>
@@ -1200,32 +1194,32 @@
         <v>17</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G8" s="2"/>
       <c r="H8" s="2" t="s">
         <v>41</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K8" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="L8" s="3" t="s">
         <v>45</v>
-      </c>
-      <c r="L8" s="3" t="s">
-        <v>46</v>
       </c>
       <c r="M8" s="2"/>
       <c r="N8" s="2"/>
       <c r="O8" s="2"/>
-      <c r="P8" s="4" t="s">
-        <v>84</v>
+      <c r="P8" s="2" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="9" spans="1:16" ht="43.5" x14ac:dyDescent="0.35">
@@ -1233,7 +1227,7 @@
         <v>12</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>18</v>
@@ -1242,32 +1236,32 @@
         <v>19</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G9" s="2"/>
       <c r="H9" s="2" t="s">
         <v>38</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K9" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="L9" s="3" t="s">
         <v>45</v>
-      </c>
-      <c r="L9" s="3" t="s">
-        <v>46</v>
       </c>
       <c r="M9" s="2"/>
       <c r="N9" s="2"/>
       <c r="O9" s="2"/>
-      <c r="P9" s="4" t="s">
-        <v>84</v>
+      <c r="P9" s="2" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="10" spans="1:16" ht="43.5" x14ac:dyDescent="0.35">
@@ -1275,7 +1269,7 @@
         <v>13</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>16</v>
@@ -1284,32 +1278,32 @@
         <v>17</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G10" s="3"/>
       <c r="H10" s="2" t="s">
         <v>41</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K10" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="L10" s="3" t="s">
         <v>45</v>
-      </c>
-      <c r="L10" s="3" t="s">
-        <v>46</v>
       </c>
       <c r="M10" s="2"/>
       <c r="N10" s="2"/>
       <c r="O10" s="2"/>
-      <c r="P10" s="4" t="s">
-        <v>84</v>
+      <c r="P10" s="2" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="11" spans="1:16" ht="43.5" x14ac:dyDescent="0.35">
@@ -1317,7 +1311,7 @@
         <v>13</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>18</v>
@@ -1326,32 +1320,32 @@
         <v>19</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="G11" s="5"/>
+        <v>117</v>
+      </c>
+      <c r="G11" s="3"/>
       <c r="H11" s="2" t="s">
         <v>38</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K11" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="L11" s="3" t="s">
         <v>45</v>
-      </c>
-      <c r="L11" s="3" t="s">
-        <v>46</v>
       </c>
       <c r="M11" s="2"/>
       <c r="N11" s="2"/>
       <c r="O11" s="2"/>
-      <c r="P11" s="4" t="s">
-        <v>84</v>
+      <c r="P11" s="2" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="12" spans="1:16" ht="43.5" x14ac:dyDescent="0.35">
@@ -1359,7 +1353,7 @@
         <v>40</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>16</v>
@@ -1368,32 +1362,32 @@
         <v>17</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G12" s="2"/>
       <c r="H12" s="2" t="s">
         <v>41</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K12" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="L12" s="3" t="s">
         <v>45</v>
-      </c>
-      <c r="L12" s="3" t="s">
-        <v>46</v>
       </c>
       <c r="M12" s="2"/>
       <c r="N12" s="2"/>
       <c r="O12" s="2"/>
-      <c r="P12" s="4" t="s">
-        <v>84</v>
+      <c r="P12" s="2" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="13" spans="1:16" ht="43.5" x14ac:dyDescent="0.35">
@@ -1401,7 +1395,7 @@
         <v>40</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>18</v>
@@ -1410,32 +1404,32 @@
         <v>19</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G13" s="2"/>
       <c r="H13" s="2" t="s">
         <v>38</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K13" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="L13" s="3" t="s">
         <v>45</v>
-      </c>
-      <c r="L13" s="3" t="s">
-        <v>46</v>
       </c>
       <c r="M13" s="2"/>
       <c r="N13" s="2"/>
       <c r="O13" s="2"/>
-      <c r="P13" s="4" t="s">
-        <v>84</v>
+      <c r="P13" s="2" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="14" spans="1:16" ht="43.5" x14ac:dyDescent="0.35">
@@ -1443,7 +1437,7 @@
         <v>14</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>16</v>
@@ -1452,32 +1446,32 @@
         <v>17</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G14" s="2"/>
       <c r="H14" s="2" t="s">
         <v>41</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K14" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="L14" s="3" t="s">
         <v>45</v>
-      </c>
-      <c r="L14" s="3" t="s">
-        <v>46</v>
       </c>
       <c r="M14" s="2"/>
       <c r="N14" s="2"/>
       <c r="O14" s="2"/>
-      <c r="P14" s="4" t="s">
-        <v>84</v>
+      <c r="P14" s="2" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="15" spans="1:16" ht="43.5" x14ac:dyDescent="0.35">
@@ -1485,7 +1479,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>18</v>
@@ -1494,32 +1488,32 @@
         <v>19</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G15" s="2"/>
       <c r="H15" s="2" t="s">
         <v>38</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K15" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="L15" s="3" t="s">
         <v>45</v>
-      </c>
-      <c r="L15" s="3" t="s">
-        <v>46</v>
       </c>
       <c r="M15" s="2"/>
       <c r="N15" s="2"/>
       <c r="O15" s="2"/>
-      <c r="P15" s="4" t="s">
-        <v>84</v>
+      <c r="P15" s="2" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="16" spans="1:16" ht="43.5" x14ac:dyDescent="0.35">
@@ -1527,7 +1521,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>16</v>
@@ -1536,32 +1530,32 @@
         <v>17</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G16" s="2"/>
       <c r="H16" s="2" t="s">
         <v>41</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K16" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="L16" s="3" t="s">
         <v>45</v>
-      </c>
-      <c r="L16" s="3" t="s">
-        <v>46</v>
       </c>
       <c r="M16" s="2"/>
       <c r="N16" s="2"/>
       <c r="O16" s="2"/>
-      <c r="P16" s="4" t="s">
-        <v>84</v>
+      <c r="P16" s="2" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="17" spans="1:16" ht="43.5" x14ac:dyDescent="0.35">
@@ -1569,7 +1563,7 @@
         <v>15</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>18</v>
@@ -1578,32 +1572,32 @@
         <v>19</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G17" s="2"/>
       <c r="H17" s="2" t="s">
         <v>38</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K17" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="L17" s="3" t="s">
         <v>45</v>
-      </c>
-      <c r="L17" s="3" t="s">
-        <v>46</v>
       </c>
       <c r="M17" s="2"/>
       <c r="N17" s="2"/>
       <c r="O17" s="2"/>
-      <c r="P17" s="4" t="s">
-        <v>84</v>
+      <c r="P17" s="2" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="18" spans="1:16" ht="43.5" x14ac:dyDescent="0.35">
@@ -1611,7 +1605,7 @@
         <v>39</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>16</v>
@@ -1620,32 +1614,32 @@
         <v>17</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G18" s="2"/>
       <c r="H18" s="2" t="s">
         <v>41</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K18" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="L18" s="3" t="s">
         <v>45</v>
-      </c>
-      <c r="L18" s="3" t="s">
-        <v>46</v>
       </c>
       <c r="M18" s="2"/>
       <c r="N18" s="2"/>
       <c r="O18" s="2"/>
-      <c r="P18" s="4" t="s">
-        <v>84</v>
+      <c r="P18" s="2" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="19" spans="1:16" ht="43.5" x14ac:dyDescent="0.35">
@@ -1653,7 +1647,7 @@
         <v>39</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>18</v>
@@ -1662,32 +1656,32 @@
         <v>19</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G19" s="2"/>
       <c r="H19" s="2" t="s">
         <v>38</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K19" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="L19" s="3" t="s">
         <v>45</v>
-      </c>
-      <c r="L19" s="3" t="s">
-        <v>46</v>
       </c>
       <c r="M19" s="2"/>
       <c r="N19" s="2"/>
       <c r="O19" s="2"/>
-      <c r="P19" s="4" t="s">
-        <v>84</v>
+      <c r="P19" s="2" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="20" spans="1:16" ht="58" x14ac:dyDescent="0.35">
@@ -1695,7 +1689,7 @@
         <v>20</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>22</v>
@@ -1704,10 +1698,10 @@
         <v>23</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G20" s="3" t="s">
         <v>36</v>
@@ -1716,22 +1710,22 @@
         <v>42</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K20" s="3" t="s">
-        <v>45</v>
+        <v>118</v>
       </c>
       <c r="L20" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="M20" s="2"/>
       <c r="N20" s="2"/>
       <c r="O20" s="2"/>
-      <c r="P20" s="4" t="s">
-        <v>84</v>
+      <c r="P20" s="2" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="21" spans="1:16" ht="58" x14ac:dyDescent="0.35">
@@ -1739,7 +1733,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>33</v>
@@ -1748,10 +1742,10 @@
         <v>34</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G21" s="3" t="s">
         <v>36</v>
@@ -1760,22 +1754,22 @@
         <v>42</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J21" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K21" s="3" t="s">
-        <v>45</v>
+        <v>118</v>
       </c>
       <c r="L21" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="M21" s="2"/>
       <c r="N21" s="2"/>
       <c r="O21" s="2"/>
-      <c r="P21" s="4" t="s">
-        <v>84</v>
+      <c r="P21" s="2" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="22" spans="1:16" ht="58" x14ac:dyDescent="0.35">
@@ -1783,7 +1777,7 @@
         <v>20</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>22</v>
@@ -1792,10 +1786,10 @@
         <v>23</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G22" s="3" t="s">
         <v>37</v>
@@ -1804,22 +1798,22 @@
         <v>42</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K22" s="3" t="s">
-        <v>45</v>
+        <v>118</v>
       </c>
       <c r="L22" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="M22" s="2"/>
       <c r="N22" s="2"/>
       <c r="O22" s="2"/>
-      <c r="P22" s="4" t="s">
-        <v>84</v>
+      <c r="P22" s="2" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="23" spans="1:16" ht="58" x14ac:dyDescent="0.35">
@@ -1827,7 +1821,7 @@
         <v>20</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>33</v>
@@ -1836,10 +1830,10 @@
         <v>34</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G23" s="3" t="s">
         <v>37</v>
@@ -1848,22 +1842,22 @@
         <v>42</v>
       </c>
       <c r="I23" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J23" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K23" s="3" t="s">
-        <v>45</v>
+        <v>118</v>
       </c>
       <c r="L23" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="M23" s="2"/>
       <c r="N23" s="2"/>
       <c r="O23" s="2"/>
-      <c r="P23" s="4" t="s">
-        <v>84</v>
+      <c r="P23" s="2" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="24" spans="1:16" ht="58" x14ac:dyDescent="0.35">
@@ -1871,7 +1865,7 @@
         <v>21</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>22</v>
@@ -1880,10 +1874,10 @@
         <v>23</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G24" s="3" t="s">
         <v>36</v>
@@ -1892,22 +1886,22 @@
         <v>42</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J24" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K24" s="3" t="s">
-        <v>45</v>
+        <v>118</v>
       </c>
       <c r="L24" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="M24" s="2"/>
       <c r="N24" s="2"/>
       <c r="O24" s="2"/>
-      <c r="P24" s="4" t="s">
-        <v>84</v>
+      <c r="P24" s="2" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="25" spans="1:16" ht="58" x14ac:dyDescent="0.35">
@@ -1915,7 +1909,7 @@
         <v>21</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>33</v>
@@ -1924,10 +1918,10 @@
         <v>34</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G25" s="3" t="s">
         <v>36</v>
@@ -1936,22 +1930,22 @@
         <v>42</v>
       </c>
       <c r="I25" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J25" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K25" s="3" t="s">
-        <v>45</v>
+        <v>118</v>
       </c>
       <c r="L25" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="M25" s="2"/>
       <c r="N25" s="2"/>
       <c r="O25" s="2"/>
-      <c r="P25" s="4" t="s">
-        <v>84</v>
+      <c r="P25" s="2" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="26" spans="1:16" ht="58" x14ac:dyDescent="0.35">
@@ -1959,7 +1953,7 @@
         <v>21</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>22</v>
@@ -1968,10 +1962,10 @@
         <v>23</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G26" s="3" t="s">
         <v>37</v>
@@ -1980,22 +1974,22 @@
         <v>42</v>
       </c>
       <c r="I26" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J26" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K26" s="3" t="s">
-        <v>45</v>
+        <v>118</v>
       </c>
       <c r="L26" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="M26" s="2"/>
       <c r="N26" s="2"/>
       <c r="O26" s="2"/>
-      <c r="P26" s="4" t="s">
-        <v>84</v>
+      <c r="P26" s="2" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="27" spans="1:16" ht="58" x14ac:dyDescent="0.35">
@@ -2003,7 +1997,7 @@
         <v>21</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>33</v>
@@ -2012,10 +2006,10 @@
         <v>34</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G27" s="3" t="s">
         <v>37</v>
@@ -2024,22 +2018,22 @@
         <v>42</v>
       </c>
       <c r="I27" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J27" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K27" s="3" t="s">
-        <v>45</v>
+        <v>118</v>
       </c>
       <c r="L27" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="M27" s="2"/>
       <c r="N27" s="2"/>
       <c r="O27" s="2"/>
-      <c r="P27" s="4" t="s">
-        <v>84</v>
+      <c r="P27" s="2" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="28" spans="1:16" ht="43.5" x14ac:dyDescent="0.35">
@@ -2047,7 +2041,7 @@
         <v>12</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>24</v>
@@ -2056,32 +2050,32 @@
         <v>17</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G28" s="2"/>
       <c r="H28" s="2" t="s">
         <v>43</v>
       </c>
       <c r="I28" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J28" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K28" s="3" t="s">
-        <v>45</v>
+        <v>118</v>
       </c>
       <c r="L28" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="M28" s="2"/>
       <c r="N28" s="2"/>
       <c r="O28" s="2"/>
-      <c r="P28" s="4" t="s">
-        <v>84</v>
+      <c r="P28" s="2" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="29" spans="1:16" ht="43.5" x14ac:dyDescent="0.35">
@@ -2089,7 +2083,7 @@
         <v>12</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>29</v>
@@ -2098,32 +2092,32 @@
         <v>19</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G29" s="2"/>
       <c r="H29" s="2" t="s">
         <v>43</v>
       </c>
       <c r="I29" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J29" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K29" s="3" t="s">
-        <v>45</v>
+        <v>118</v>
       </c>
       <c r="L29" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="M29" s="2"/>
       <c r="N29" s="2"/>
       <c r="O29" s="2"/>
-      <c r="P29" s="4" t="s">
-        <v>84</v>
+      <c r="P29" s="2" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="30" spans="1:16" ht="43.5" x14ac:dyDescent="0.35">
@@ -2131,7 +2125,7 @@
         <v>12</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>35</v>
@@ -2140,32 +2134,32 @@
         <v>19</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G30" s="2"/>
       <c r="H30" s="2" t="s">
         <v>43</v>
       </c>
       <c r="I30" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J30" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K30" s="3" t="s">
-        <v>45</v>
+        <v>118</v>
       </c>
       <c r="L30" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="M30" s="2"/>
       <c r="N30" s="2"/>
       <c r="O30" s="2"/>
-      <c r="P30" s="4" t="s">
-        <v>84</v>
+      <c r="P30" s="2" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="31" spans="1:16" ht="43.5" x14ac:dyDescent="0.35">
@@ -2173,7 +2167,7 @@
         <v>26</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>24</v>
@@ -2182,32 +2176,32 @@
         <v>17</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G31" s="2"/>
       <c r="H31" s="2" t="s">
         <v>43</v>
       </c>
       <c r="I31" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J31" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K31" s="3" t="s">
-        <v>45</v>
+        <v>118</v>
       </c>
       <c r="L31" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="M31" s="2"/>
       <c r="N31" s="2"/>
       <c r="O31" s="2"/>
-      <c r="P31" s="4" t="s">
-        <v>84</v>
+      <c r="P31" s="2" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="32" spans="1:16" ht="43.5" x14ac:dyDescent="0.35">
@@ -2215,7 +2209,7 @@
         <v>26</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>29</v>
@@ -2224,32 +2218,32 @@
         <v>19</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G32" s="2"/>
       <c r="H32" s="2" t="s">
         <v>43</v>
       </c>
       <c r="I32" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J32" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K32" s="3" t="s">
-        <v>45</v>
+        <v>118</v>
       </c>
       <c r="L32" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="M32" s="2"/>
       <c r="N32" s="2"/>
       <c r="O32" s="2"/>
-      <c r="P32" s="4" t="s">
-        <v>84</v>
+      <c r="P32" s="2" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="33" spans="1:16" ht="43.5" x14ac:dyDescent="0.35">
@@ -2257,7 +2251,7 @@
         <v>26</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>35</v>
@@ -2266,32 +2260,32 @@
         <v>19</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G33" s="2"/>
       <c r="H33" s="2" t="s">
         <v>43</v>
       </c>
       <c r="I33" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J33" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K33" s="3" t="s">
-        <v>45</v>
+        <v>118</v>
       </c>
       <c r="L33" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="M33" s="2"/>
       <c r="N33" s="2"/>
       <c r="O33" s="2"/>
-      <c r="P33" s="4" t="s">
-        <v>84</v>
+      <c r="P33" s="2" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="34" spans="1:16" ht="43.5" x14ac:dyDescent="0.35">
@@ -2299,7 +2293,7 @@
         <v>25</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>24</v>
@@ -2308,32 +2302,32 @@
         <v>17</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G34" s="2"/>
       <c r="H34" s="2" t="s">
         <v>43</v>
       </c>
       <c r="I34" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J34" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K34" s="3" t="s">
-        <v>45</v>
+        <v>118</v>
       </c>
       <c r="L34" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="M34" s="2"/>
       <c r="N34" s="2"/>
       <c r="O34" s="2"/>
-      <c r="P34" s="4" t="s">
-        <v>84</v>
+      <c r="P34" s="2" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="35" spans="1:16" ht="43.5" x14ac:dyDescent="0.35">
@@ -2341,7 +2335,7 @@
         <v>25</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>29</v>
@@ -2350,32 +2344,32 @@
         <v>19</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G35" s="2"/>
       <c r="H35" s="2" t="s">
         <v>43</v>
       </c>
       <c r="I35" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J35" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K35" s="3" t="s">
-        <v>45</v>
+        <v>118</v>
       </c>
       <c r="L35" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="M35" s="2"/>
       <c r="N35" s="2"/>
       <c r="O35" s="2"/>
-      <c r="P35" s="4" t="s">
-        <v>84</v>
+      <c r="P35" s="2" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="36" spans="1:16" ht="43.5" x14ac:dyDescent="0.35">
@@ -2383,7 +2377,7 @@
         <v>25</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>35</v>
@@ -2392,32 +2386,32 @@
         <v>19</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G36" s="2"/>
       <c r="H36" s="2" t="s">
         <v>43</v>
       </c>
       <c r="I36" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J36" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K36" s="3" t="s">
-        <v>45</v>
+        <v>118</v>
       </c>
       <c r="L36" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="M36" s="2"/>
       <c r="N36" s="2"/>
       <c r="O36" s="2"/>
-      <c r="P36" s="4" t="s">
-        <v>84</v>
+      <c r="P36" s="2" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="37" spans="1:16" ht="43.5" x14ac:dyDescent="0.35">
@@ -2425,7 +2419,7 @@
         <v>27</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>24</v>
@@ -2434,32 +2428,32 @@
         <v>17</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G37" s="2"/>
       <c r="H37" s="2" t="s">
         <v>43</v>
       </c>
       <c r="I37" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J37" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K37" s="3" t="s">
-        <v>45</v>
+        <v>118</v>
       </c>
       <c r="L37" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="M37" s="2"/>
       <c r="N37" s="2"/>
       <c r="O37" s="2"/>
-      <c r="P37" s="4" t="s">
-        <v>84</v>
+      <c r="P37" s="2" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="38" spans="1:16" ht="43.5" x14ac:dyDescent="0.35">
@@ -2467,7 +2461,7 @@
         <v>27</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>29</v>
@@ -2476,32 +2470,32 @@
         <v>19</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G38" s="2"/>
       <c r="H38" s="2" t="s">
         <v>43</v>
       </c>
       <c r="I38" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J38" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K38" s="3" t="s">
-        <v>45</v>
+        <v>118</v>
       </c>
       <c r="L38" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="M38" s="2"/>
       <c r="N38" s="2"/>
       <c r="O38" s="2"/>
-      <c r="P38" s="4" t="s">
-        <v>84</v>
+      <c r="P38" s="2" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="39" spans="1:16" ht="43.5" x14ac:dyDescent="0.35">
@@ -2509,7 +2503,7 @@
         <v>27</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>35</v>
@@ -2518,32 +2512,32 @@
         <v>19</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G39" s="2"/>
       <c r="H39" s="2" t="s">
         <v>43</v>
       </c>
       <c r="I39" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J39" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K39" s="3" t="s">
-        <v>45</v>
+        <v>118</v>
       </c>
       <c r="L39" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="M39" s="2"/>
       <c r="N39" s="2"/>
       <c r="O39" s="2"/>
-      <c r="P39" s="4" t="s">
-        <v>84</v>
+      <c r="P39" s="2" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="40" spans="1:16" ht="43.5" x14ac:dyDescent="0.35">
@@ -2551,7 +2545,7 @@
         <v>28</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C40" s="2" t="s">
         <v>24</v>
@@ -2560,32 +2554,32 @@
         <v>17</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G40" s="2"/>
       <c r="H40" s="2" t="s">
         <v>43</v>
       </c>
       <c r="I40" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J40" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K40" s="3" t="s">
-        <v>45</v>
+        <v>118</v>
       </c>
       <c r="L40" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="M40" s="2"/>
       <c r="N40" s="2"/>
       <c r="O40" s="2"/>
-      <c r="P40" s="4" t="s">
-        <v>84</v>
+      <c r="P40" s="2" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="41" spans="1:16" ht="43.5" x14ac:dyDescent="0.35">
@@ -2593,7 +2587,7 @@
         <v>28</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C41" s="2" t="s">
         <v>29</v>
@@ -2602,32 +2596,32 @@
         <v>19</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F41" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G41" s="2"/>
       <c r="H41" s="2" t="s">
         <v>43</v>
       </c>
       <c r="I41" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J41" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K41" s="3" t="s">
-        <v>45</v>
+        <v>118</v>
       </c>
       <c r="L41" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="M41" s="2"/>
       <c r="N41" s="2"/>
       <c r="O41" s="2"/>
-      <c r="P41" s="4" t="s">
-        <v>84</v>
+      <c r="P41" s="2" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="42" spans="1:16" ht="43.5" x14ac:dyDescent="0.35">
@@ -2635,7 +2629,7 @@
         <v>28</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C42" s="2" t="s">
         <v>35</v>
@@ -2644,32 +2638,32 @@
         <v>19</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F42" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G42" s="2"/>
       <c r="H42" s="2" t="s">
         <v>43</v>
       </c>
       <c r="I42" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J42" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K42" s="3" t="s">
-        <v>45</v>
+        <v>118</v>
       </c>
       <c r="L42" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="M42" s="2"/>
       <c r="N42" s="2"/>
       <c r="O42" s="2"/>
-      <c r="P42" s="4" t="s">
-        <v>84</v>
+      <c r="P42" s="2" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="43" spans="1:16" ht="43.5" x14ac:dyDescent="0.35">
@@ -2677,36 +2671,36 @@
         <v>30</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C43" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D43" s="2" t="s">
         <v>70</v>
-      </c>
-      <c r="D43" s="2" t="s">
-        <v>71</v>
       </c>
       <c r="E43" s="2"/>
       <c r="F43" s="2"/>
       <c r="G43" s="2"/>
       <c r="H43" s="2"/>
       <c r="I43" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J43" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K43" s="3" t="s">
-        <v>45</v>
+        <v>118</v>
       </c>
       <c r="L43" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="M43" s="2"/>
       <c r="O43" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="P43" s="4" t="s">
-        <v>84</v>
+        <v>74</v>
+      </c>
+      <c r="P43" s="2" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="44" spans="1:16" ht="43.5" x14ac:dyDescent="0.35">
@@ -2714,7 +2708,7 @@
         <v>30</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C44" s="2" t="s">
         <v>35</v>
@@ -2727,23 +2721,23 @@
       <c r="G44" s="2"/>
       <c r="H44" s="2"/>
       <c r="I44" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J44" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K44" s="3" t="s">
-        <v>45</v>
+        <v>118</v>
       </c>
       <c r="L44" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="M44" s="2"/>
       <c r="O44" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="P44" s="4" t="s">
-        <v>84</v>
+        <v>74</v>
+      </c>
+      <c r="P44" s="2" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="45" spans="1:16" ht="43.5" x14ac:dyDescent="0.35">
@@ -2751,36 +2745,36 @@
         <v>30</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C45" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D45" s="2" t="s">
         <v>72</v>
-      </c>
-      <c r="D45" s="2" t="s">
-        <v>73</v>
       </c>
       <c r="E45" s="2"/>
       <c r="F45" s="2"/>
       <c r="G45" s="2"/>
       <c r="H45" s="2"/>
       <c r="I45" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J45" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K45" s="3" t="s">
-        <v>45</v>
+        <v>118</v>
       </c>
       <c r="L45" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="M45" s="2"/>
       <c r="O45" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="P45" s="4" t="s">
-        <v>84</v>
+        <v>74</v>
+      </c>
+      <c r="P45" s="2" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="46" spans="1:16" ht="43.5" x14ac:dyDescent="0.35">
@@ -2789,33 +2783,33 @@
       </c>
       <c r="B46" s="2"/>
       <c r="C46" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D46" s="2" t="s">
         <v>70</v>
-      </c>
-      <c r="D46" s="2" t="s">
-        <v>71</v>
       </c>
       <c r="E46" s="2"/>
       <c r="F46" s="2"/>
       <c r="G46" s="2"/>
       <c r="H46" s="2"/>
       <c r="I46" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J46" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K46" s="3" t="s">
-        <v>45</v>
+        <v>118</v>
       </c>
       <c r="L46" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="M46" s="2"/>
       <c r="O46" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="P46" s="4" t="s">
-        <v>84</v>
+        <v>75</v>
+      </c>
+      <c r="P46" s="2" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="47" spans="1:16" ht="43.5" x14ac:dyDescent="0.35">
@@ -2834,23 +2828,23 @@
       <c r="G47" s="2"/>
       <c r="H47" s="2"/>
       <c r="I47" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J47" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K47" s="3" t="s">
-        <v>45</v>
+        <v>118</v>
       </c>
       <c r="L47" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="M47" s="2"/>
       <c r="O47" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="P47" s="4" t="s">
-        <v>84</v>
+        <v>75</v>
+      </c>
+      <c r="P47" s="2" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="48" spans="1:16" ht="43.5" x14ac:dyDescent="0.35">
@@ -2859,33 +2853,33 @@
       </c>
       <c r="B48" s="2"/>
       <c r="C48" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D48" s="2" t="s">
         <v>72</v>
-      </c>
-      <c r="D48" s="2" t="s">
-        <v>73</v>
       </c>
       <c r="E48" s="2"/>
       <c r="F48" s="2"/>
       <c r="G48" s="2"/>
       <c r="H48" s="2"/>
       <c r="I48" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J48" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K48" s="3" t="s">
-        <v>45</v>
+        <v>118</v>
       </c>
       <c r="L48" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="M48" s="2"/>
       <c r="O48" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="P48" s="4" t="s">
-        <v>84</v>
+        <v>75</v>
+      </c>
+      <c r="P48" s="2" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="49" spans="1:16" ht="43.5" x14ac:dyDescent="0.35">
@@ -2893,42 +2887,42 @@
         <v>32</v>
       </c>
       <c r="B49" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C49" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="C49" s="2" t="s">
+      <c r="D49" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="D49" s="2" t="s">
-        <v>71</v>
-      </c>
       <c r="E49" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F49" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G49" s="2"/>
       <c r="H49" s="2" t="s">
         <v>44</v>
       </c>
       <c r="I49" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J49" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K49" s="3" t="s">
-        <v>45</v>
+        <v>118</v>
       </c>
       <c r="L49" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="M49" s="2"/>
       <c r="O49" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="P49" s="4" t="s">
-        <v>84</v>
+        <v>73</v>
+      </c>
+      <c r="P49" s="2" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="50" spans="1:16" ht="43.5" x14ac:dyDescent="0.35">
@@ -2936,7 +2930,7 @@
         <v>32</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C50" s="2" t="s">
         <v>35</v>
@@ -2945,33 +2939,33 @@
         <v>19</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F50" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G50" s="2"/>
       <c r="H50" s="2" t="s">
         <v>44</v>
       </c>
       <c r="I50" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J50" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K50" s="3" t="s">
-        <v>45</v>
+        <v>118</v>
       </c>
       <c r="L50" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="M50" s="2"/>
       <c r="O50" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="P50" s="4" t="s">
-        <v>84</v>
+        <v>73</v>
+      </c>
+      <c r="P50" s="2" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="51" spans="1:16" ht="43.5" x14ac:dyDescent="0.35">
@@ -2979,42 +2973,42 @@
         <v>32</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C51" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D51" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="D51" s="2" t="s">
-        <v>73</v>
-      </c>
       <c r="E51" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F51" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G51" s="2"/>
       <c r="H51" s="2" t="s">
         <v>44</v>
       </c>
       <c r="I51" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J51" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K51" s="3" t="s">
-        <v>45</v>
+        <v>118</v>
       </c>
       <c r="L51" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="M51" s="2"/>
       <c r="O51" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="P51" s="4" t="s">
-        <v>84</v>
+        <v>73</v>
+      </c>
+      <c r="P51" s="2" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="52" spans="1:16" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
In the column variables change " " to "_"
</commit_message>
<xml_diff>
--- a/buehlot/metadata.xlsx
+++ b/buehlot/metadata.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\flori\Documents\GitHub\scripts\buehlot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6898B68-DF87-4D27-AD32-5954237A76B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64B5BA4D-4B56-4553-BB60-3F1241D73364}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -112,9 +112,6 @@
     <t>uwe.ehret@kit.edu</t>
   </si>
   <si>
-    <t>air temperature</t>
-  </si>
-  <si>
     <t>°C</t>
   </si>
   <si>
@@ -230,9 +227,6 @@
     <t>28.13.01_01.01_01</t>
   </si>
   <si>
-    <t>bulk electrical conductivity</t>
-  </si>
-  <si>
     <t>dS/m</t>
   </si>
   <si>
@@ -252,9 +246,6 @@
     <t xml:space="preserve">A soil moisture meter has sensors for two variables, one for the electrical conductivity and one for the volumetric water content. Each station has two different depths where the variables are being collected. </t>
   </si>
   <si>
-    <t>volumetric water content</t>
-  </si>
-  <si>
     <t>28.13.01_01.01_02</t>
   </si>
   <si>
@@ -271,9 +262,6 @@
   </si>
   <si>
     <t>28.13.01_01.05_04</t>
-  </si>
-  <si>
-    <t>ground water level</t>
   </si>
   <si>
     <t xml:space="preserve">3440517.80
@@ -287,12 +275,6 @@
   </si>
   <si>
     <t>A tensiometer has sensors for three variables, the ground water level, the logger temperature and the water temperater. The meters are located in different areas to collect the data.</t>
-  </si>
-  <si>
-    <t>logger temperature</t>
-  </si>
-  <si>
-    <t>water temperature</t>
   </si>
   <si>
     <t xml:space="preserve">3440517.80
@@ -523,6 +505,24 @@
   </si>
   <si>
     <t>data/data_export/water_temperature/Sprengquellen_unten_süd_water_temperature</t>
+  </si>
+  <si>
+    <t>air_temperature</t>
+  </si>
+  <si>
+    <t>bulk_electrical_conductivity</t>
+  </si>
+  <si>
+    <t>volumetric_water_content</t>
+  </si>
+  <si>
+    <t>ground_water_level</t>
+  </si>
+  <si>
+    <t>logger_temperature</t>
+  </si>
+  <si>
+    <t>water_temperature</t>
   </si>
 </sst>
 </file>
@@ -995,8 +995,8 @@
   <dimension ref="A1:R75"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="65" zoomScaleNormal="65" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="R5" sqref="R5"/>
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1032,7 +1032,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>4</v>
@@ -1071,7 +1071,7 @@
         <v>15</v>
       </c>
       <c r="R1" s="4" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
     </row>
     <row r="2" spans="1:18" ht="43.5" x14ac:dyDescent="0.35">
@@ -1088,7 +1088,7 @@
         <v>19</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>20</v>
@@ -1119,7 +1119,7 @@
         <v>27</v>
       </c>
       <c r="R2" s="5" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
     </row>
     <row r="3" spans="1:18" ht="43.5" x14ac:dyDescent="0.35">
@@ -1130,13 +1130,13 @@
         <v>17</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>29</v>
-      </c>
       <c r="E3" s="2" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>20</v>
@@ -1146,7 +1146,7 @@
       </c>
       <c r="H3" s="2"/>
       <c r="I3" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J3" s="2" t="s">
         <v>23</v>
@@ -1167,15 +1167,15 @@
         <v>27</v>
       </c>
       <c r="R3" s="5" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
     </row>
     <row r="4" spans="1:18" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>31</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>32</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>18</v>
@@ -1184,13 +1184,13 @@
         <v>19</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="F4" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G4" s="3" t="s">
         <v>33</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>34</v>
       </c>
       <c r="H4" s="2"/>
       <c r="I4" s="2" t="s">
@@ -1215,34 +1215,34 @@
         <v>27</v>
       </c>
       <c r="R4" s="5" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
     </row>
     <row r="5" spans="1:18" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="C5" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="F5" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="F5" s="3" t="s">
+      <c r="G5" s="3" t="s">
         <v>33</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>34</v>
       </c>
       <c r="H5" s="2"/>
       <c r="I5" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J5" s="2" t="s">
         <v>23</v>
@@ -1263,15 +1263,15 @@
         <v>27</v>
       </c>
       <c r="R5" s="2" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
     </row>
     <row r="6" spans="1:18" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>35</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>36</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>18</v>
@@ -1280,13 +1280,13 @@
         <v>19</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="F6" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="G6" s="3" t="s">
         <v>37</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>38</v>
       </c>
       <c r="H6" s="2"/>
       <c r="I6" s="2" t="s">
@@ -1311,34 +1311,34 @@
         <v>27</v>
       </c>
       <c r="R6" s="5" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
     </row>
     <row r="7" spans="1:18" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="C7" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="F7" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="F7" s="3" t="s">
+      <c r="G7" s="3" t="s">
         <v>37</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>38</v>
       </c>
       <c r="H7" s="2"/>
       <c r="I7" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J7" s="2" t="s">
         <v>23</v>
@@ -1359,15 +1359,15 @@
         <v>27</v>
       </c>
       <c r="R7" s="5" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
     </row>
     <row r="8" spans="1:18" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>39</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>40</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>18</v>
@@ -1376,13 +1376,13 @@
         <v>19</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="F8" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="G8" s="3" t="s">
         <v>41</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>42</v>
       </c>
       <c r="H8" s="2"/>
       <c r="I8" s="2" t="s">
@@ -1407,34 +1407,34 @@
         <v>27</v>
       </c>
       <c r="R8" s="5" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
     </row>
     <row r="9" spans="1:18" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="C9" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="F9" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="C9" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="F9" s="3" t="s">
+      <c r="G9" s="3" t="s">
         <v>41</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>42</v>
       </c>
       <c r="H9" s="2"/>
       <c r="I9" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J9" s="2" t="s">
         <v>23</v>
@@ -1455,15 +1455,15 @@
         <v>27</v>
       </c>
       <c r="R9" s="5" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
     </row>
     <row r="10" spans="1:18" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>43</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>44</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>18</v>
@@ -1472,13 +1472,13 @@
         <v>19</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="F10" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="G10" s="3" t="s">
         <v>45</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>46</v>
       </c>
       <c r="H10" s="3"/>
       <c r="I10" s="2" t="s">
@@ -1503,34 +1503,34 @@
         <v>27</v>
       </c>
       <c r="R10" s="5" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
     </row>
     <row r="11" spans="1:18" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="C11" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="F11" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="C11" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="F11" s="3" t="s">
+      <c r="G11" s="3" t="s">
         <v>45</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>46</v>
       </c>
       <c r="H11" s="3"/>
       <c r="I11" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J11" s="2" t="s">
         <v>23</v>
@@ -1551,15 +1551,15 @@
         <v>27</v>
       </c>
       <c r="R11" s="5" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
     </row>
     <row r="12" spans="1:18" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>18</v>
@@ -1568,13 +1568,13 @@
         <v>19</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="F12" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="G12" s="3" t="s">
         <v>48</v>
-      </c>
-      <c r="G12" s="3" t="s">
-        <v>49</v>
       </c>
       <c r="H12" s="2"/>
       <c r="I12" s="2" t="s">
@@ -1599,34 +1599,34 @@
         <v>27</v>
       </c>
       <c r="R12" s="5" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
     </row>
     <row r="13" spans="1:18" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="B13" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="F13" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="C13" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="F13" s="3" t="s">
+      <c r="G13" s="3" t="s">
         <v>48</v>
-      </c>
-      <c r="G13" s="3" t="s">
-        <v>49</v>
       </c>
       <c r="H13" s="2"/>
       <c r="I13" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J13" s="2" t="s">
         <v>23</v>
@@ -1647,15 +1647,15 @@
         <v>27</v>
       </c>
       <c r="R13" s="5" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
     </row>
     <row r="14" spans="1:18" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>50</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>51</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>18</v>
@@ -1664,13 +1664,13 @@
         <v>19</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="F14" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="G14" s="3" t="s">
         <v>52</v>
-      </c>
-      <c r="G14" s="3" t="s">
-        <v>53</v>
       </c>
       <c r="H14" s="2"/>
       <c r="I14" s="2" t="s">
@@ -1695,34 +1695,34 @@
         <v>27</v>
       </c>
       <c r="R14" s="5" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
     </row>
     <row r="15" spans="1:18" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="C15" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="F15" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="C15" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="F15" s="3" t="s">
+      <c r="G15" s="3" t="s">
         <v>52</v>
-      </c>
-      <c r="G15" s="3" t="s">
-        <v>53</v>
       </c>
       <c r="H15" s="2"/>
       <c r="I15" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J15" s="2" t="s">
         <v>23</v>
@@ -1743,15 +1743,15 @@
         <v>27</v>
       </c>
       <c r="R15" s="5" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
     </row>
     <row r="16" spans="1:18" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>54</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>55</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>18</v>
@@ -1760,13 +1760,13 @@
         <v>19</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="F16" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="G16" s="3" t="s">
         <v>56</v>
-      </c>
-      <c r="G16" s="3" t="s">
-        <v>57</v>
       </c>
       <c r="H16" s="2"/>
       <c r="I16" s="2" t="s">
@@ -1791,34 +1791,34 @@
         <v>27</v>
       </c>
       <c r="R16" s="5" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
     </row>
     <row r="17" spans="1:18" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="B17" s="2" t="s">
-        <v>55</v>
-      </c>
       <c r="C17" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="D17" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="D17" s="2" t="s">
-        <v>29</v>
-      </c>
       <c r="E17" s="2" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H17" s="2"/>
       <c r="I17" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J17" s="2" t="s">
         <v>23</v>
@@ -1839,15 +1839,15 @@
         <v>27</v>
       </c>
       <c r="R17" s="5" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
     </row>
     <row r="18" spans="1:18" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>18</v>
@@ -1856,13 +1856,13 @@
         <v>19</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="F18" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="G18" s="3" t="s">
         <v>60</v>
-      </c>
-      <c r="G18" s="3" t="s">
-        <v>61</v>
       </c>
       <c r="H18" s="2"/>
       <c r="I18" s="2" t="s">
@@ -1887,34 +1887,34 @@
         <v>27</v>
       </c>
       <c r="R18" s="5" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
     </row>
     <row r="19" spans="1:18" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="B19" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="F19" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="C19" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="F19" s="3" t="s">
+      <c r="G19" s="3" t="s">
         <v>60</v>
-      </c>
-      <c r="G19" s="3" t="s">
-        <v>61</v>
       </c>
       <c r="H19" s="2"/>
       <c r="I19" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J19" s="2" t="s">
         <v>23</v>
@@ -1935,48 +1935,48 @@
         <v>27</v>
       </c>
       <c r="R19" s="5" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
     </row>
     <row r="20" spans="1:18" ht="58" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B20" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="C20" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="D20" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="E20" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="F20" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="D20" s="2" t="s">
+      <c r="G20" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="E20" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="F20" s="3" t="s">
+      <c r="H20" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="G20" s="3" t="s">
+      <c r="I20" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="H20" s="3" t="s">
+      <c r="J20" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K20" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L20" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="M20" s="3" t="s">
         <v>68</v>
-      </c>
-      <c r="I20" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="J20" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="K20" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="L20" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="M20" s="3" t="s">
-        <v>70</v>
       </c>
       <c r="N20" s="2"/>
       <c r="O20" s="2"/>
@@ -1985,48 +1985,48 @@
         <v>27</v>
       </c>
       <c r="R20" s="5" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
     </row>
     <row r="21" spans="1:18" ht="58" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B21" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="B21" s="2" t="s">
-        <v>63</v>
-      </c>
       <c r="C21" s="2" t="s">
-        <v>71</v>
+        <v>145</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="F21" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="G21" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="H21" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="G21" s="3" t="s">
+      <c r="I21" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="H21" s="3" t="s">
+      <c r="J21" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K21" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L21" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="M21" s="3" t="s">
         <v>68</v>
-      </c>
-      <c r="I21" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="J21" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="K21" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="L21" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="M21" s="3" t="s">
-        <v>70</v>
       </c>
       <c r="N21" s="2"/>
       <c r="O21" s="2"/>
@@ -2035,37 +2035,37 @@
         <v>27</v>
       </c>
       <c r="R21" s="5" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
     </row>
     <row r="22" spans="1:18" ht="58" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C22" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="F22" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="D22" s="2" t="s">
+      <c r="G22" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="E22" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="F22" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="G22" s="3" t="s">
+      <c r="H22" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="I22" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="H22" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="I22" s="2" t="s">
-        <v>69</v>
-      </c>
       <c r="J22" s="2" t="s">
         <v>23</v>
       </c>
@@ -2076,7 +2076,7 @@
         <v>25</v>
       </c>
       <c r="M22" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="N22" s="2"/>
       <c r="O22" s="2"/>
@@ -2085,37 +2085,37 @@
         <v>27</v>
       </c>
       <c r="R22" s="5" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
     </row>
     <row r="23" spans="1:18" ht="58" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>71</v>
+        <v>145</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G23" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="H23" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="I23" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="H23" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="I23" s="2" t="s">
-        <v>69</v>
-      </c>
       <c r="J23" s="2" t="s">
         <v>23</v>
       </c>
@@ -2126,7 +2126,7 @@
         <v>25</v>
       </c>
       <c r="M23" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="N23" s="2"/>
       <c r="O23" s="2"/>
@@ -2135,48 +2135,48 @@
         <v>27</v>
       </c>
       <c r="R23" s="5" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
     </row>
     <row r="24" spans="1:18" ht="58" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>64</v>
+        <v>144</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="F24" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="G24" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="G24" s="3" t="s">
-        <v>42</v>
-      </c>
       <c r="H24" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="I24" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="J24" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K24" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L24" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="M24" s="3" t="s">
         <v>68</v>
-      </c>
-      <c r="I24" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="J24" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="K24" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="L24" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="M24" s="3" t="s">
-        <v>70</v>
       </c>
       <c r="N24" s="2"/>
       <c r="O24" s="2"/>
@@ -2185,48 +2185,48 @@
         <v>27</v>
       </c>
       <c r="R24" s="5" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
     </row>
     <row r="25" spans="1:18" ht="58" x14ac:dyDescent="0.35">
       <c r="A25" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>71</v>
+        <v>145</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="F25" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="G25" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="G25" s="3" t="s">
-        <v>42</v>
-      </c>
       <c r="H25" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="I25" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="J25" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K25" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L25" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="M25" s="3" t="s">
         <v>68</v>
-      </c>
-      <c r="I25" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="J25" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="K25" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="L25" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="M25" s="3" t="s">
-        <v>70</v>
       </c>
       <c r="N25" s="2"/>
       <c r="O25" s="2"/>
@@ -2235,36 +2235,36 @@
         <v>27</v>
       </c>
       <c r="R25" s="5" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
     </row>
     <row r="26" spans="1:18" ht="58" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>64</v>
+        <v>144</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="F26" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="G26" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="G26" s="3" t="s">
-        <v>42</v>
-      </c>
       <c r="H26" s="3" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="I26" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="J26" s="2" t="s">
         <v>23</v>
@@ -2276,7 +2276,7 @@
         <v>25</v>
       </c>
       <c r="M26" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="N26" s="2"/>
       <c r="O26" s="2"/>
@@ -2285,36 +2285,36 @@
         <v>27</v>
       </c>
       <c r="R26" s="5" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
     </row>
     <row r="27" spans="1:18" ht="58" x14ac:dyDescent="0.35">
       <c r="A27" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>71</v>
+        <v>145</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="F27" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="G27" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="G27" s="3" t="s">
-        <v>42</v>
-      </c>
       <c r="H27" s="3" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="I27" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="J27" s="2" t="s">
         <v>23</v>
@@ -2326,7 +2326,7 @@
         <v>25</v>
       </c>
       <c r="M27" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="N27" s="2"/>
       <c r="O27" s="2"/>
@@ -2335,34 +2335,34 @@
         <v>27</v>
       </c>
       <c r="R27" s="5" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
     </row>
     <row r="28" spans="1:18" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A28" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>78</v>
+        <v>146</v>
       </c>
       <c r="D28" s="2" t="s">
         <v>19</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="H28" s="2"/>
       <c r="I28" s="2" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="J28" s="2" t="s">
         <v>23</v>
@@ -2374,7 +2374,7 @@
         <v>25</v>
       </c>
       <c r="M28" s="3" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="N28" s="2"/>
       <c r="O28" s="2"/>
@@ -2383,34 +2383,34 @@
         <v>27</v>
       </c>
       <c r="R28" s="5" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
     </row>
     <row r="29" spans="1:18" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A29" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>83</v>
+        <v>147</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="H29" s="2"/>
       <c r="I29" s="2" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="J29" s="2" t="s">
         <v>23</v>
@@ -2422,7 +2422,7 @@
         <v>25</v>
       </c>
       <c r="M29" s="3" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="N29" s="2"/>
       <c r="O29" s="2"/>
@@ -2431,34 +2431,34 @@
         <v>27</v>
       </c>
       <c r="R29" s="5" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
     </row>
     <row r="30" spans="1:18" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A30" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>84</v>
+        <v>148</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="H30" s="2"/>
       <c r="I30" s="2" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="J30" s="2" t="s">
         <v>23</v>
@@ -2470,7 +2470,7 @@
         <v>25</v>
       </c>
       <c r="M30" s="3" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="N30" s="2"/>
       <c r="O30" s="2"/>
@@ -2479,34 +2479,34 @@
         <v>27</v>
       </c>
       <c r="R30" s="5" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
     </row>
     <row r="31" spans="1:18" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A31" s="2" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>78</v>
+        <v>146</v>
       </c>
       <c r="D31" s="2" t="s">
         <v>19</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="H31" s="2"/>
       <c r="I31" s="2" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="J31" s="2" t="s">
         <v>23</v>
@@ -2518,7 +2518,7 @@
         <v>25</v>
       </c>
       <c r="M31" s="3" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="N31" s="2"/>
       <c r="O31" s="2"/>
@@ -2527,34 +2527,34 @@
         <v>27</v>
       </c>
       <c r="R31" s="5" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
     </row>
     <row r="32" spans="1:18" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A32" s="2" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="C32" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="F32" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="G32" s="3" t="s">
         <v>83</v>
-      </c>
-      <c r="D32" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="E32" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="F32" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="G32" s="3" t="s">
-        <v>89</v>
       </c>
       <c r="H32" s="2"/>
       <c r="I32" s="2" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="J32" s="2" t="s">
         <v>23</v>
@@ -2566,7 +2566,7 @@
         <v>25</v>
       </c>
       <c r="M32" s="3" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="N32" s="2"/>
       <c r="O32" s="2"/>
@@ -2575,34 +2575,34 @@
         <v>27</v>
       </c>
       <c r="R32" s="5" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
     </row>
     <row r="33" spans="1:18" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A33" s="2" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>84</v>
+        <v>148</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="H33" s="2"/>
       <c r="I33" s="2" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="J33" s="2" t="s">
         <v>23</v>
@@ -2614,7 +2614,7 @@
         <v>25</v>
       </c>
       <c r="M33" s="3" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="N33" s="2"/>
       <c r="O33" s="2"/>
@@ -2623,34 +2623,34 @@
         <v>27</v>
       </c>
       <c r="R33" s="5" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
     </row>
     <row r="34" spans="1:18" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A34" s="2" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>78</v>
+        <v>146</v>
       </c>
       <c r="D34" s="2" t="s">
         <v>19</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="H34" s="2"/>
       <c r="I34" s="2" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="J34" s="2" t="s">
         <v>23</v>
@@ -2662,7 +2662,7 @@
         <v>25</v>
       </c>
       <c r="M34" s="3" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="N34" s="2"/>
       <c r="O34" s="2"/>
@@ -2671,34 +2671,34 @@
         <v>27</v>
       </c>
       <c r="R34" s="5" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
     </row>
     <row r="35" spans="1:18" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A35" s="2" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>83</v>
+        <v>147</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="H35" s="2"/>
       <c r="I35" s="2" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="J35" s="2" t="s">
         <v>23</v>
@@ -2710,7 +2710,7 @@
         <v>25</v>
       </c>
       <c r="M35" s="3" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="N35" s="2"/>
       <c r="O35" s="2"/>
@@ -2719,34 +2719,34 @@
         <v>27</v>
       </c>
       <c r="R35" s="5" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
     </row>
     <row r="36" spans="1:18" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A36" s="2" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>84</v>
+        <v>148</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="H36" s="2"/>
       <c r="I36" s="2" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="J36" s="2" t="s">
         <v>23</v>
@@ -2758,7 +2758,7 @@
         <v>25</v>
       </c>
       <c r="M36" s="3" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="N36" s="2"/>
       <c r="O36" s="2"/>
@@ -2767,34 +2767,34 @@
         <v>27</v>
       </c>
       <c r="R36" s="5" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
     </row>
     <row r="37" spans="1:18" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A37" s="2" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>78</v>
+        <v>146</v>
       </c>
       <c r="D37" s="2" t="s">
         <v>19</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="G37" s="3" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="H37" s="2"/>
       <c r="I37" s="2" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="J37" s="2" t="s">
         <v>23</v>
@@ -2806,7 +2806,7 @@
         <v>25</v>
       </c>
       <c r="M37" s="3" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="N37" s="2"/>
       <c r="O37" s="2"/>
@@ -2815,34 +2815,34 @@
         <v>27</v>
       </c>
       <c r="R37" s="5" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
     </row>
     <row r="38" spans="1:18" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A38" s="2" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>83</v>
+        <v>147</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="H38" s="2"/>
       <c r="I38" s="2" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="J38" s="2" t="s">
         <v>23</v>
@@ -2854,7 +2854,7 @@
         <v>25</v>
       </c>
       <c r="M38" s="3" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="N38" s="2"/>
       <c r="O38" s="2"/>
@@ -2863,34 +2863,34 @@
         <v>27</v>
       </c>
       <c r="R38" s="5" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
     </row>
     <row r="39" spans="1:18" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A39" s="2" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>84</v>
+        <v>148</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="G39" s="3" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="H39" s="2"/>
       <c r="I39" s="2" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="J39" s="2" t="s">
         <v>23</v>
@@ -2902,7 +2902,7 @@
         <v>25</v>
       </c>
       <c r="M39" s="3" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="N39" s="2"/>
       <c r="O39" s="2"/>
@@ -2911,34 +2911,34 @@
         <v>27</v>
       </c>
       <c r="R39" s="5" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
     </row>
     <row r="40" spans="1:18" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A40" s="2" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>78</v>
+        <v>146</v>
       </c>
       <c r="D40" s="2" t="s">
         <v>19</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="G40" s="3" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="H40" s="2"/>
       <c r="I40" s="2" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="J40" s="2" t="s">
         <v>23</v>
@@ -2950,7 +2950,7 @@
         <v>25</v>
       </c>
       <c r="M40" s="3" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="N40" s="2"/>
       <c r="O40" s="2"/>
@@ -2959,34 +2959,34 @@
         <v>27</v>
       </c>
       <c r="R40" s="5" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
     </row>
     <row r="41" spans="1:18" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A41" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E41" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="B41" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="C41" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="D41" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="E41" s="2" t="s">
-        <v>103</v>
-      </c>
       <c r="F41" s="3" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="G41" s="3" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="H41" s="2"/>
       <c r="I41" s="2" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="J41" s="2" t="s">
         <v>23</v>
@@ -2998,7 +2998,7 @@
         <v>25</v>
       </c>
       <c r="M41" s="3" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="N41" s="2"/>
       <c r="O41" s="2"/>
@@ -3007,34 +3007,34 @@
         <v>27</v>
       </c>
       <c r="R41" s="5" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
     </row>
     <row r="42" spans="1:18" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A42" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E42" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="B42" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="C42" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="D42" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="E42" s="2" t="s">
-        <v>103</v>
-      </c>
       <c r="F42" s="3" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="G42" s="3" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="H42" s="2"/>
       <c r="I42" s="2" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="J42" s="2" t="s">
         <v>23</v>
@@ -3046,7 +3046,7 @@
         <v>25</v>
       </c>
       <c r="M42" s="3" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="N42" s="2"/>
       <c r="O42" s="2"/>
@@ -3055,7 +3055,7 @@
         <v>27</v>
       </c>
       <c r="R42" s="5" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
     </row>
     <row r="43" spans="1:18" x14ac:dyDescent="0.35">

</xml_diff>